<commit_message>
Agrego Vf al lazo de corriente y los tb para medir el pmos del Buck
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Documents\Carpeta de Agus\FIUBA\Cursadas\2022 1erC\Diseño de circuitos electrónicos\Proyecto\Git\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49C4B0F-CD15-430B-88A2-3A75A597BBDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D2DCC8-E39B-4281-BC8B-1EE7D3733762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Estabilidad LDO" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
   <si>
     <t>Característica</t>
   </si>
@@ -336,6 +337,21 @@
   </si>
   <si>
     <t>VB creciendo, SELA=1    VB creciendo, SELA=0</t>
+  </si>
+  <si>
+    <t>Peor caso lazo tensión</t>
+  </si>
+  <si>
+    <t>RL = 250</t>
+  </si>
+  <si>
+    <t>CL = 15uF</t>
+  </si>
+  <si>
+    <t>P2 = 22.8kHz</t>
+  </si>
+  <si>
+    <t>Queda:</t>
   </si>
 </sst>
 </file>
@@ -684,19 +700,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -719,7 +735,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -730,7 +746,7 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
@@ -751,7 +767,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -768,7 +784,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -785,7 +801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -800,7 +816,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
@@ -817,7 +833,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -832,7 +848,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>25</v>
       </c>
@@ -843,7 +859,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -854,7 +870,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -871,7 +887,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
@@ -888,7 +904,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -905,7 +921,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -922,7 +938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -937,7 +953,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -952,7 +968,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -969,7 +985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>46</v>
       </c>
@@ -986,7 +1002,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1001,7 +1017,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1012,7 +1028,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>56</v>
       </c>
@@ -1029,7 +1045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>57</v>
@@ -1044,7 +1060,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>60</v>
       </c>
@@ -1059,7 +1075,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>62</v>
       </c>
@@ -1076,7 +1092,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>63</v>
@@ -1091,7 +1107,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>66</v>
       </c>
@@ -1106,7 +1122,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -1123,7 +1139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -1142,7 +1158,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>76</v>
       </c>
@@ -1159,7 +1175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>77</v>
       </c>
@@ -1176,7 +1192,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>78</v>
       </c>
@@ -1193,7 +1209,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>79</v>
@@ -1208,7 +1224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>80</v>
       </c>
@@ -1225,7 +1241,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>81</v>
@@ -1240,7 +1256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>84</v>
       </c>
@@ -1257,7 +1273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>86</v>
@@ -1272,7 +1288,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>89</v>
       </c>
@@ -1289,7 +1305,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>93</v>
@@ -1304,7 +1320,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>90</v>
       </c>
@@ -1321,7 +1337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>95</v>
@@ -1336,7 +1352,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>91</v>
       </c>
@@ -1353,7 +1369,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>96</v>
@@ -1368,7 +1384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1377,7 +1393,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1386,7 +1402,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1395,7 +1411,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1404,7 +1420,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1413,7 +1429,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1422,7 +1438,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1431,7 +1447,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1440,7 +1456,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1449,7 +1465,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1458,7 +1474,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1467,7 +1483,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1476,7 +1492,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1485,7 +1501,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1494,7 +1510,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1503,7 +1519,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1512,7 +1528,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1521,7 +1537,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1530,7 +1546,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1539,7 +1555,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1548,7 +1564,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1557,7 +1573,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1566,7 +1582,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1575,7 +1591,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1603,4 +1619,44 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6880DA-5A0C-4D13-A01A-1C906D80BF23}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Agregados archivos de Monte Carlo
</commit_message>
<xml_diff>
--- a/Especificaciones.xlsx
+++ b/Especificaciones.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Documents\GitHub\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agust\Documents\Carpeta de Agus\FIUBA\Cursadas\2022 1erC\Diseño de circuitos electrónicos\Proyecto\Git\DISE-O_CIRCUITOS_ELECTRONICOS_1C_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D2DCC8-E39B-4281-BC8B-1EE7D3733762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BDEF43-2C1F-4358-8190-3D26FE29D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Estabilidad LDO" sheetId="2" r:id="rId2"/>
+    <sheet name="Generales" sheetId="1" r:id="rId1"/>
+    <sheet name="Montecarlo" sheetId="3" r:id="rId2"/>
+    <sheet name="Peor Caso" sheetId="4" r:id="rId3"/>
+    <sheet name="Estabilidad LDO" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="105">
   <si>
     <t>Característica</t>
   </si>
@@ -395,7 +397,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -403,19 +405,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -700,42 +720,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="7" max="7" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -746,120 +766,120 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
         <v>12</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>24</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>36</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>26</v>
       </c>
@@ -870,154 +890,154 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
         <v>200</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1" t="s">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1" t="s">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>55</v>
       </c>
@@ -1028,363 +1048,363 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:7" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="1" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1" t="s">
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="1" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1" t="s">
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
         <v>750</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1" t="s">
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
         <v>200</v>
       </c>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1" t="s">
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
         <v>1.5</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1" t="s">
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
         <v>400</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="s">
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1" t="s">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="1" t="s">
+    <row r="32" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1" t="s">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="1" t="s">
+    <row r="34" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1" t="s">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="1" t="s">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C36" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="1" t="s">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="1" t="s">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="1" t="s">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1393,7 +1413,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1402,7 +1422,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1411,7 +1431,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1420,7 +1440,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1429,7 +1449,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1438,7 +1458,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1447,7 +1467,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1456,7 +1476,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1465,7 +1485,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1474,7 +1494,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1483,7 +1503,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1492,7 +1512,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1501,7 +1521,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1510,7 +1530,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1519,7 +1539,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1528,7 +1548,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1537,7 +1557,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1546,7 +1566,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1555,7 +1575,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1564,7 +1584,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1573,7 +1593,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1582,7 +1602,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1591,7 +1611,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1622,36 +1642,756 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1551953A-29A8-4B20-AD45-C2045503F788}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2">
+        <v>36</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2">
+        <v>200</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="4"/>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2">
+        <v>750</v>
+      </c>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2">
+        <v>200</v>
+      </c>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2">
+        <v>400</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A34" s="4"/>
+      <c r="B34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="4"/>
+      <c r="B36" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="4"/>
+      <c r="B38" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="4"/>
+      <c r="B40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BDC0545-EEFA-4D35-8FD3-2D3A03F24621}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6880DA-5A0C-4D13-A01A-1C906D80BF23}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>103</v>
       </c>

</xml_diff>